<commit_message>
Filter by PLS-DA first version The datasets can be filtered according to the loadings of the PLS-DA analysis and the result will be saved in a excel sheet.
</commit_message>
<xml_diff>
--- a/data-raw/testdata/labels.xlsx
+++ b/data-raw/testdata/labels.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\workspace\Holomics\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\workspace\Holomics\data-raw\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D67C4BBB-602B-4389-AA41-22A0912D9A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC36BCD-B290-4EFA-B192-8B31A4D69A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D82AE664-C31C-46C4-A0C3-A6C76EDA62EC}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{D82AE664-C31C-46C4-A0C3-A6C76EDA62EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -48,10 +48,10 @@
     <t>Colorcode</t>
   </si>
   <si>
-    <t>#445566</t>
+    <t>#f54266</t>
   </si>
   <si>
-    <t>#993422</t>
+    <t>#42f548</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed classes file format and reformated code The file with classes now needs to contain the sample names in the first row and before performing the analysis it is checked if the data and the classes file contain the same sample names.
</commit_message>
<xml_diff>
--- a/data-raw/testdata/labels.xlsx
+++ b/data-raw/testdata/labels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\workspace\Holomics\data-raw\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katha\AIT\Holomics\data-raw\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC36BCD-B290-4EFA-B192-8B31A4D69A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CEF192-FA57-4839-88D9-78CB3C9EF5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{D82AE664-C31C-46C4-A0C3-A6C76EDA62EC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D82AE664-C31C-46C4-A0C3-A6C76EDA62EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
   <si>
     <t>Storability</t>
   </si>
@@ -52,6 +52,57 @@
   </si>
   <si>
     <t>#42f548</t>
+  </si>
+  <si>
+    <t>Samples</t>
+  </si>
+  <si>
+    <t>V1_1_t0</t>
+  </si>
+  <si>
+    <t>V1_2_t0</t>
+  </si>
+  <si>
+    <t>V1_3_t0</t>
+  </si>
+  <si>
+    <t>V1_4_t0</t>
+  </si>
+  <si>
+    <t>V2_1_t0</t>
+  </si>
+  <si>
+    <t>V2_2_t0</t>
+  </si>
+  <si>
+    <t>V2_3_t0</t>
+  </si>
+  <si>
+    <t>V2_4_t0</t>
+  </si>
+  <si>
+    <t>V5_1_t0</t>
+  </si>
+  <si>
+    <t>V5_2_t0</t>
+  </si>
+  <si>
+    <t>V5_3_t0</t>
+  </si>
+  <si>
+    <t>V5_4_t0</t>
+  </si>
+  <si>
+    <t>V6_1_t0</t>
+  </si>
+  <si>
+    <t>V6_2_t0</t>
+  </si>
+  <si>
+    <t>V6_3_t0</t>
+  </si>
+  <si>
+    <t>V6_4_t0</t>
   </si>
 </sst>
 </file>
@@ -416,147 +467,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA3BA68-DFFC-4961-9910-FF42755D1F87}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>